<commit_message>
Inaccurate Case Code pushed
</commit_message>
<xml_diff>
--- a/src/test/testdata/Test_Case_R3_Report.xlsx
+++ b/src/test/testdata/Test_Case_R3_Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R3_Report_Automation\src\test\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R3_Project\R3_Report_Automation\src\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081BAAB9-4F24-46D6-8CDB-56F543AA2B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA3D866-118B-4F61-83BC-35CA73F2D424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2855E3E2-C5F0-4EF0-BC43-ED693B49271B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Test Steps</t>
   </si>
@@ -65,25 +65,19 @@
     <t>Selvamani_M</t>
   </si>
   <si>
-    <t>0000_ORG_PROV_Phone_Scenario</t>
-  </si>
-  <si>
-    <t>Verify the Accurate bucket for ORG_PROV_Phone Info</t>
-  </si>
-  <si>
-    <t>Verify_Accurate_Bucket_ORG_PROV_Phone</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
     <t>No. of R3 Excel Row's to Execute</t>
   </si>
   <si>
-    <t>1 to 3</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>0000_ORG_Phone_Scenario</t>
+  </si>
+  <si>
+    <t>Verify the ORG_Phone Info</t>
+  </si>
+  <si>
+    <t>Verify_All_Buckets_ORG_PHONE</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -485,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6498BC77-3AA9-4CBF-B796-9F71168359A9}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,14 +491,13 @@
     <col min="2" max="2" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -515,44 +508,38 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="G2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Accurate and Inaccurate Case for OV UseCase code is done
</commit_message>
<xml_diff>
--- a/src/test/testdata/Test_Case_R3_Report.xlsx
+++ b/src/test/testdata/Test_Case_R3_Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R3_Project\R3_Report_Automation\src\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA3D866-118B-4F61-83BC-35CA73F2D424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9776AB-9C72-49A5-ABB9-F0959F2F2514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2855E3E2-C5F0-4EF0-BC43-ED693B49271B}"/>
   </bookViews>
@@ -77,7 +77,7 @@
     <t>Verify_All_Buckets_ORG_PHONE</t>
   </si>
   <si>
-    <t>100</t>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -183,9 +183,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -223,7 +223,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -329,7 +329,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -471,7 +471,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -482,7 +482,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Scenario 3.1 case: PV accurate ORG level initial code is done
</commit_message>
<xml_diff>
--- a/src/test/testdata/Test_Case_R3_Report.xlsx
+++ b/src/test/testdata/Test_Case_R3_Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R3_Project\R3_Report_Automation\src\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9776AB-9C72-49A5-ABB9-F0959F2F2514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB64B55A-786E-44EC-B760-B5AA6B08F687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2855E3E2-C5F0-4EF0-BC43-ED693B49271B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Test Steps</t>
   </si>
@@ -77,7 +77,34 @@
     <t>Verify_All_Buckets_ORG_PHONE</t>
   </si>
   <si>
-    <t>8</t>
+    <t>0000_ORG_PV_Phone_Scenario</t>
+  </si>
+  <si>
+    <t>Verify the ORG_PV_Phone Info</t>
+  </si>
+  <si>
+    <t>Verify_All_Buckets_ORG_PV_PHONE</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0000_ORG_Website_Cache_Scenario</t>
+  </si>
+  <si>
+    <t>Verify the ORG_Website_Cache_ Info</t>
+  </si>
+  <si>
+    <t>Verify_ORG_WEBSITE_CACHE</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -183,9 +210,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -223,7 +250,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -329,7 +356,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -471,7 +498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -479,15 +506,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6498BC77-3AA9-4CBF-B796-9F71168359A9}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" style="1" customWidth="1"/>
@@ -531,15 +558,61 @@
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>